<commit_message>
add face color task
</commit_message>
<xml_diff>
--- a/preproc/Psych_FaceSwitch.xlsx
+++ b/preproc/Psych_FaceSwitch.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\test\EphysAnalysis_FaceSwitch_New\preproc_face_switch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\FaceSwitch\code\EphysAnalysis_FaceSwitch\preproc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31663D03-0B41-4380-A515-70AEDB35635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D900A267-E82C-496E-B7C0-96E46F21274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{9E121B91-0AB2-4816-96BF-262F0B6EB626}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="344">
   <si>
     <t>valid</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1021,6 +1021,284 @@
   </si>
   <si>
     <t>Nick20250613_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20250819/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20250820/</t>
+  </si>
+  <si>
+    <t>20250821/</t>
+  </si>
+  <si>
+    <t>20250822/</t>
+  </si>
+  <si>
+    <t>20250823/</t>
+  </si>
+  <si>
+    <t>20250825/</t>
+  </si>
+  <si>
+    <t>20250826/</t>
+  </si>
+  <si>
+    <t>20250827/</t>
+  </si>
+  <si>
+    <t>20250828/</t>
+  </si>
+  <si>
+    <t>20250829/</t>
+  </si>
+  <si>
+    <t>20250830/</t>
+  </si>
+  <si>
+    <t>20250901/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20250902/</t>
+  </si>
+  <si>
+    <t>20250903/</t>
+  </si>
+  <si>
+    <t>20250904/</t>
+  </si>
+  <si>
+    <t>20250905/</t>
+  </si>
+  <si>
+    <t>20250906/</t>
+  </si>
+  <si>
+    <t>20250908/</t>
+  </si>
+  <si>
+    <t>20250909/</t>
+  </si>
+  <si>
+    <t>Nick20250819_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250820_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250821_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250822_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250823_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250825_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250826_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250827_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250828_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250829_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250830_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250901_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250902_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250903_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250904_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250905_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250906_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250908_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250909_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250819_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250820_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250821_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250822_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250823_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250825_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250826_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250827_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250828_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250829_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250830_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250901_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250902_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250903_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250904_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250905_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250906_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250908_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250909_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>faceColor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bad performance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overfed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20250910/</t>
+  </si>
+  <si>
+    <t>20250911/</t>
+  </si>
+  <si>
+    <t>20250912/</t>
+  </si>
+  <si>
+    <t>20250913/</t>
+  </si>
+  <si>
+    <t>20250914/</t>
+  </si>
+  <si>
+    <t>Nick20250910_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250911_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250912_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250913_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250914_01.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250910_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250911_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250912_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250913_01_eye.mat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nick20250914_01_eye.mat</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1154,7 +1432,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1186,6 +1464,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1258,8 +1542,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0860E63E-D433-47B0-8DBE-F7C474B5A6C5}" name="表1" displayName="表1" ref="A1:L82" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="A1:L82" xr:uid="{0860E63E-D433-47B0-8DBE-F7C474B5A6C5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0860E63E-D433-47B0-8DBE-F7C474B5A6C5}" name="表1" displayName="表1" ref="A1:L110" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A1:L110" xr:uid="{0860E63E-D433-47B0-8DBE-F7C474B5A6C5}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{489E95F9-2631-4FA3-9EBF-B582E0EDAC40}" name="raw_folder" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{5383F5E2-1CAD-4D49-8711-B48ABC62C858}" name="formatted_folder" dataDxfId="10"/>
@@ -1575,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68E046B-ABF3-42AA-9D06-07A510DCAFC5}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M99" sqref="M99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4105,6 +4389,756 @@
         <v>94</v>
       </c>
     </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+      <c r="K88" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="H89" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="H93" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>